<commit_message>
test case for sdl-6761 on iot env
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\data-layer-automation\src\main\resources\test-data-xls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1BF83E-F107-4973-A5F9-4410760134F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E6277C-8881-4975-BC40-1F2EA53E83C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="5" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-14560" windowWidth="38620" windowHeight="21220" tabRatio="800" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -24,9 +24,10 @@
     <sheet name="deleteEntities" sheetId="4" r:id="rId9"/>
     <sheet name="createRelations" sheetId="19" r:id="rId10"/>
     <sheet name="updateRelations" sheetId="20" r:id="rId11"/>
-    <sheet name="getRelationById" sheetId="7" r:id="rId12"/>
-    <sheet name="getRelations" sheetId="6" r:id="rId13"/>
-    <sheet name="deleteRelations" sheetId="16" r:id="rId14"/>
+    <sheet name="listGraphNames" sheetId="24" r:id="rId12"/>
+    <sheet name="getRelationById" sheetId="7" r:id="rId13"/>
+    <sheet name="getRelations" sheetId="6" r:id="rId14"/>
+    <sheet name="deleteRelations" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="392">
   <si>
     <t>testEntity1</t>
   </si>
@@ -3852,35 +3853,51 @@
     <t>snc-entityMgmt-publishCheck-update-Test-22</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>iot-lpg-list-graph-names</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>list all graph names</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>response</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>[ "janusgraph_iot_demo_dev_kg",   "janusgraph_iot_demo_dev_instance_kg"]</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -3933,7 +3950,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3987,6 +4004,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4275,7 +4295,7 @@
       <selection activeCell="W5" sqref="W5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="21" max="21" width="60.5546875" customWidth="1"/>
     <col min="22" max="22" width="48.21875" customWidth="1"/>
@@ -4283,7 +4303,7 @@
     <col min="28" max="28" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="21:28">
+    <row r="1" spans="21:28" x14ac:dyDescent="0.25">
       <c r="U1" s="9" t="s">
         <v>7</v>
       </c>
@@ -4309,7 +4329,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="21:28" ht="409.6">
+    <row r="2" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U2" s="10" t="s">
         <v>231</v>
       </c>
@@ -4331,7 +4351,7 @@
       <c r="AA2" s="19"/>
       <c r="AB2" s="5"/>
     </row>
-    <row r="3" spans="21:28" ht="409.6">
+    <row r="3" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U3" s="10" t="s">
         <v>233</v>
       </c>
@@ -4355,7 +4375,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="21:28" ht="409.6">
+    <row r="4" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U4" s="10" t="s">
         <v>238</v>
       </c>
@@ -4379,7 +4399,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="21:28" ht="409.6">
+    <row r="5" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U5" s="10" t="s">
         <v>241</v>
       </c>
@@ -4403,7 +4423,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="6" spans="21:28" ht="409.6">
+    <row r="6" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U6" s="10" t="s">
         <v>245</v>
       </c>
@@ -4425,7 +4445,7 @@
       <c r="AA6" s="5"/>
       <c r="AB6" s="5"/>
     </row>
-    <row r="7" spans="21:28" ht="409.6">
+    <row r="7" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U7" s="10" t="s">
         <v>248</v>
       </c>
@@ -4449,7 +4469,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="8" spans="21:28" ht="409.6">
+    <row r="8" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U8" s="10" t="s">
         <v>252</v>
       </c>
@@ -4471,7 +4491,7 @@
       <c r="AA8" s="5"/>
       <c r="AB8" s="5"/>
     </row>
-    <row r="9" spans="21:28" ht="409.6">
+    <row r="9" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U9" s="10" t="s">
         <v>255</v>
       </c>
@@ -4495,7 +4515,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="10" spans="21:28" ht="409.6">
+    <row r="10" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U10" s="10" t="s">
         <v>258</v>
       </c>
@@ -4517,7 +4537,7 @@
       <c r="AA10" s="5"/>
       <c r="AB10" s="5"/>
     </row>
-    <row r="11" spans="21:28" ht="409.6">
+    <row r="11" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U11" s="10" t="s">
         <v>261</v>
       </c>
@@ -4539,7 +4559,7 @@
       <c r="AA11" s="5"/>
       <c r="AB11" s="5"/>
     </row>
-    <row r="12" spans="21:28" ht="409.6">
+    <row r="12" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U12" s="10" t="s">
         <v>264</v>
       </c>
@@ -4563,7 +4583,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="13" spans="21:28" ht="409.6">
+    <row r="13" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U13" s="10" t="s">
         <v>268</v>
       </c>
@@ -4587,7 +4607,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="14" spans="21:28" ht="409.6">
+    <row r="14" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U14" s="10" t="s">
         <v>272</v>
       </c>
@@ -4611,7 +4631,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="15" spans="21:28" ht="409.6">
+    <row r="15" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U15" s="10" t="s">
         <v>275</v>
       </c>
@@ -4635,7 +4655,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="16" spans="21:28" ht="409.6">
+    <row r="16" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U16" s="10" t="s">
         <v>278</v>
       </c>
@@ -4657,7 +4677,7 @@
       <c r="AA16" s="5"/>
       <c r="AB16" s="5"/>
     </row>
-    <row r="17" spans="21:28" ht="409.6">
+    <row r="17" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U17" s="10" t="s">
         <v>281</v>
       </c>
@@ -4679,7 +4699,7 @@
       <c r="AA17" s="5"/>
       <c r="AB17" s="5"/>
     </row>
-    <row r="18" spans="21:28" ht="409.6">
+    <row r="18" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U18" s="10" t="s">
         <v>284</v>
       </c>
@@ -4703,7 +4723,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="21:28" ht="409.6">
+    <row r="19" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U19" s="10" t="s">
         <v>287</v>
       </c>
@@ -4727,7 +4747,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="21:28" ht="409.6">
+    <row r="20" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U20" s="10" t="s">
         <v>290</v>
       </c>
@@ -4751,7 +4771,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="21:28" ht="409.6">
+    <row r="21" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U21" s="10" t="s">
         <v>293</v>
       </c>
@@ -4775,7 +4795,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="21:28" ht="409.6">
+    <row r="22" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U22" s="10" t="s">
         <v>297</v>
       </c>
@@ -4799,7 +4819,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="23" spans="21:28" ht="409.6">
+    <row r="23" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U23" s="10" t="s">
         <v>301</v>
       </c>
@@ -4823,7 +4843,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="24" spans="21:28" ht="409.6">
+    <row r="24" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U24" s="10" t="s">
         <v>304</v>
       </c>
@@ -4846,7 +4866,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="25" spans="21:28" ht="409.6">
+    <row r="25" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U25" s="10" t="s">
         <v>308</v>
       </c>
@@ -4869,7 +4889,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="26" spans="21:28" ht="409.6">
+    <row r="26" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U26" s="10" t="s">
         <v>312</v>
       </c>
@@ -4889,7 +4909,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="27" spans="21:28" ht="409.6">
+    <row r="27" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U27" s="10" t="s">
         <v>315</v>
       </c>
@@ -4909,7 +4929,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="28" spans="21:28" ht="409.6">
+    <row r="28" spans="21:28" ht="409.6" x14ac:dyDescent="0.25">
       <c r="U28" s="10" t="s">
         <v>318</v>
       </c>
@@ -4945,7 +4965,7 @@
       <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.109375" style="5" bestFit="1" customWidth="1"/>
@@ -4960,7 +4980,7 @@
     <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +5012,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="111" customHeight="1">
+    <row r="2" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -5020,7 +5040,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="7"/>
     </row>
-    <row r="3" spans="1:10" ht="111" customHeight="1">
+    <row r="3" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>60</v>
       </c>
@@ -5042,7 +5062,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="7"/>
     </row>
-    <row r="4" spans="1:10" ht="111" customHeight="1">
+    <row r="4" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -5064,7 +5084,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="7"/>
     </row>
-    <row r="5" spans="1:10" ht="111" customHeight="1">
+    <row r="5" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>62</v>
       </c>
@@ -5086,7 +5106,7 @@
       <c r="I5" s="6"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" ht="111" customHeight="1">
+    <row r="6" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>63</v>
       </c>
@@ -5108,7 +5128,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="7"/>
     </row>
-    <row r="7" spans="1:10" ht="111" customHeight="1">
+    <row r="7" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>64</v>
       </c>
@@ -5130,7 +5150,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="111" customHeight="1">
+    <row r="8" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>65</v>
       </c>
@@ -5156,7 +5176,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="111" customHeight="1">
+    <row r="9" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>66</v>
       </c>
@@ -5182,7 +5202,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="111" customHeight="1">
+    <row r="10" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>67</v>
       </c>
@@ -5208,7 +5228,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="111" customHeight="1">
+    <row r="11" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>153</v>
       </c>
@@ -5234,7 +5254,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="111" customHeight="1">
+    <row r="12" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>154</v>
       </c>
@@ -5260,7 +5280,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="111" customHeight="1">
+    <row r="13" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>155</v>
       </c>
@@ -5286,7 +5306,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="111" customHeight="1">
+    <row r="14" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>156</v>
       </c>
@@ -5312,7 +5332,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="111" customHeight="1">
+    <row r="15" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>157</v>
       </c>
@@ -5338,7 +5358,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="111" customHeight="1">
+    <row r="16" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>173</v>
       </c>
@@ -5364,7 +5384,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="111" customHeight="1">
+    <row r="17" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>174</v>
       </c>
@@ -5390,7 +5410,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="111" customHeight="1">
+    <row r="18" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>183</v>
       </c>
@@ -5416,7 +5436,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="111" customHeight="1">
+    <row r="19" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>184</v>
       </c>
@@ -5442,7 +5462,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="111" customHeight="1">
+    <row r="20" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
         <v>185</v>
       </c>
@@ -5468,7 +5488,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="111" customHeight="1">
+    <row r="21" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>186</v>
       </c>
@@ -5494,7 +5514,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="111" customHeight="1">
+    <row r="22" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>187</v>
       </c>
@@ -5520,7 +5540,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="111" customHeight="1">
+    <row r="23" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>191</v>
       </c>
@@ -5546,7 +5566,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="111" customHeight="1">
+    <row r="24" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
         <v>200</v>
       </c>
@@ -5572,7 +5592,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="111" customHeight="1">
+    <row r="25" spans="1:10" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>207</v>
       </c>
@@ -5609,11 +5629,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1F5FE0E-8788-403D-8502-6CD26A71119B}">
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.77734375" style="14" bestFit="1" customWidth="1"/>
@@ -5629,7 +5649,7 @@
     <col min="12" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -5664,7 +5684,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="106.2" customHeight="1">
+    <row r="2" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -5695,7 +5715,7 @@
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
     </row>
-    <row r="3" spans="1:11" ht="106.2" customHeight="1">
+    <row r="3" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
@@ -5718,7 +5738,7 @@
       <c r="J3" s="6"/>
       <c r="K3" s="6"/>
     </row>
-    <row r="4" spans="1:11" ht="106.2" customHeight="1">
+    <row r="4" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -5745,7 +5765,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="106.2" customHeight="1">
+    <row r="5" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
@@ -5772,7 +5792,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="106.2" customHeight="1">
+    <row r="6" spans="1:11" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -5809,6 +5829,68 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23BC73A-A0BF-4177-B9E9-728F3C997D3D}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" s="2">
+        <v>200</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -5816,7 +5898,7 @@
       <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.77734375" style="14" bestFit="1" customWidth="1"/>
@@ -5830,7 +5912,7 @@
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -5859,7 +5941,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="303.60000000000002">
+    <row r="2" spans="1:9" ht="316.8" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>70</v>
       </c>
@@ -5888,7 +5970,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="27.6">
+    <row r="3" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>72</v>
       </c>
@@ -5911,7 +5993,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27.6">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>73</v>
       </c>
@@ -5941,7 +6023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7825D-C3D3-4455-B765-0D831E376750}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -5949,7 +6031,7 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="29.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.44140625" style="1" bestFit="1" customWidth="1"/>
@@ -5960,7 +6042,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -5980,7 +6062,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>75</v>
       </c>
@@ -5998,7 +6080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>76</v>
       </c>
@@ -6018,7 +6100,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>77</v>
       </c>
@@ -6038,7 +6120,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>78</v>
       </c>
@@ -6065,7 +6147,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -6073,7 +6155,7 @@
       <selection activeCell="G4" sqref="G4:I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.77734375" style="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.109375" style="18" bestFit="1" customWidth="1"/>
@@ -6087,7 +6169,7 @@
     <col min="10" max="16384" width="8.77734375" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
@@ -6116,7 +6198,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="148.19999999999999" customHeight="1">
+    <row r="2" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
         <v>79</v>
       </c>
@@ -6145,7 +6227,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="148.19999999999999" customHeight="1">
+    <row r="3" spans="1:9" ht="148.19999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>80</v>
       </c>
@@ -6172,7 +6254,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="27.6">
+    <row r="4" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>81</v>
       </c>
@@ -6195,7 +6277,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="27.6">
+    <row r="5" spans="1:9" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>83</v>
       </c>
@@ -6233,7 +6315,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="72.33203125" customWidth="1"/>
     <col min="4" max="4" width="31.5546875" customWidth="1"/>
@@ -6241,7 +6323,7 @@
     <col min="8" max="8" width="109.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="27.6">
+    <row r="1" spans="1:8" ht="26.4" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -6267,7 +6349,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6">
+    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>324</v>
       </c>
@@ -6308,7 +6390,7 @@
       <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.33203125" customWidth="1"/>
     <col min="2" max="2" width="78.88671875" customWidth="1"/>
@@ -6317,7 +6399,7 @@
     <col min="8" max="8" width="35.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -6343,7 +6425,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="409.6">
+    <row r="2" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>328</v>
       </c>
@@ -6365,7 +6447,7 @@
       <c r="G2" s="19"/>
       <c r="H2" s="5"/>
     </row>
-    <row r="3" spans="1:8" ht="409.6">
+    <row r="3" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>341</v>
       </c>
@@ -6388,7 +6470,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="409.6">
+    <row r="4" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>343</v>
       </c>
@@ -6411,7 +6493,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="216">
+    <row r="5" spans="1:8" ht="207" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>369</v>
       </c>
@@ -6434,7 +6516,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="244.8">
+    <row r="6" spans="1:8" ht="234.6" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>370</v>
       </c>
@@ -6457,7 +6539,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="409.6">
+    <row r="7" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>371</v>
       </c>
@@ -6480,7 +6562,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="409.6">
+    <row r="8" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>372</v>
       </c>
@@ -6500,7 +6582,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="409.6">
+    <row r="9" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>373</v>
       </c>
@@ -6520,7 +6602,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="409.6">
+    <row r="10" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>374</v>
       </c>
@@ -6543,7 +6625,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="409.6">
+    <row r="11" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>375</v>
       </c>
@@ -6566,7 +6648,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="409.6">
+    <row r="12" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>376</v>
       </c>
@@ -6589,7 +6671,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="409.6">
+    <row r="13" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>377</v>
       </c>
@@ -6612,7 +6694,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="409.6">
+    <row r="14" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>378</v>
       </c>
@@ -6632,7 +6714,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="409.6">
+    <row r="15" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>379</v>
       </c>
@@ -6652,7 +6734,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="409.6">
+    <row r="16" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>380</v>
       </c>
@@ -6675,7 +6757,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="409.6">
+    <row r="17" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>381</v>
       </c>
@@ -6698,7 +6780,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="409.6">
+    <row r="18" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>382</v>
       </c>
@@ -6721,7 +6803,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="409.6">
+    <row r="19" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>383</v>
       </c>
@@ -6744,7 +6826,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="409.6">
+    <row r="20" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>384</v>
       </c>
@@ -6767,7 +6849,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="409.6">
+    <row r="21" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
         <v>385</v>
       </c>
@@ -6790,7 +6872,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="409.6">
+    <row r="22" spans="1:8" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A22" s="10" t="s">
         <v>386</v>
       </c>
@@ -6813,7 +6895,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="216">
+    <row r="23" spans="1:8" ht="207" x14ac:dyDescent="0.25">
       <c r="A23" s="10" t="s">
         <v>387</v>
       </c>
@@ -6852,7 +6934,7 @@
       <selection pane="bottomLeft" activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.44140625" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.44140625" style="14" bestFit="1" customWidth="1"/>
@@ -6866,7 +6948,7 @@
     <col min="10" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -6895,7 +6977,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="106.2" customHeight="1">
+    <row r="2" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
@@ -6920,7 +7002,7 @@
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
     </row>
-    <row r="3" spans="1:9" ht="106.2" customHeight="1">
+    <row r="3" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>20</v>
       </c>
@@ -6941,7 +7023,7 @@
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
     </row>
-    <row r="4" spans="1:9" ht="106.2" customHeight="1">
+    <row r="4" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
@@ -6962,7 +7044,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" spans="1:9" ht="106.2" customHeight="1">
+    <row r="5" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>22</v>
       </c>
@@ -6983,7 +7065,7 @@
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
     </row>
-    <row r="6" spans="1:9" ht="106.2" customHeight="1">
+    <row r="6" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>23</v>
       </c>
@@ -7008,7 +7090,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="106.2" customHeight="1">
+    <row r="7" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>24</v>
       </c>
@@ -7033,7 +7115,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="106.2" customHeight="1">
+    <row r="8" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
         <v>25</v>
       </c>
@@ -7058,7 +7140,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="106.2" customHeight="1">
+    <row r="9" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
         <v>91</v>
       </c>
@@ -7083,7 +7165,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="106.2" customHeight="1">
+    <row r="10" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
         <v>92</v>
       </c>
@@ -7108,7 +7190,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="106.2" customHeight="1">
+    <row r="11" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>93</v>
       </c>
@@ -7133,7 +7215,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="106.2" customHeight="1">
+    <row r="12" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="10" t="s">
         <v>110</v>
       </c>
@@ -7158,7 +7240,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="106.2" customHeight="1">
+    <row r="13" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
         <v>111</v>
       </c>
@@ -7183,7 +7265,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="106.2" customHeight="1">
+    <row r="14" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
         <v>112</v>
       </c>
@@ -7208,7 +7290,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="106.2" customHeight="1">
+    <row r="15" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
         <v>117</v>
       </c>
@@ -7233,7 +7315,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="106.2" customHeight="1">
+    <row r="16" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
         <v>118</v>
       </c>
@@ -7258,7 +7340,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="106.2" customHeight="1">
+    <row r="17" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>119</v>
       </c>
@@ -7283,7 +7365,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="106.2" customHeight="1">
+    <row r="18" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
         <v>120</v>
       </c>
@@ -7308,7 +7390,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="106.2" customHeight="1">
+    <row r="19" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>121</v>
       </c>
@@ -7333,7 +7415,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="106.2" customHeight="1">
+    <row r="20" spans="1:9" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>122</v>
       </c>
@@ -7373,7 +7455,7 @@
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.109375" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.33203125" style="14" bestFit="1" customWidth="1"/>
@@ -7388,7 +7470,7 @@
     <col min="11" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -7420,7 +7502,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="106.2" customHeight="1">
+    <row r="2" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>26</v>
       </c>
@@ -7448,7 +7530,7 @@
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
     </row>
-    <row r="3" spans="1:10" ht="106.2" customHeight="1">
+    <row r="3" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>27</v>
       </c>
@@ -7470,7 +7552,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="106.2" customHeight="1">
+    <row r="4" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>30</v>
       </c>
@@ -7496,7 +7578,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="106.2" customHeight="1">
+    <row r="5" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>31</v>
       </c>
@@ -7522,7 +7604,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="106.2" customHeight="1">
+    <row r="6" spans="1:10" ht="106.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>32</v>
       </c>
@@ -7565,7 +7647,7 @@
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" style="5" bestFit="1" customWidth="1"/>
@@ -7578,7 +7660,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
@@ -7604,7 +7686,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.6">
+    <row r="2" spans="1:8" ht="171.6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>38</v>
       </c>
@@ -7630,7 +7712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -7652,7 +7734,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
@@ -7686,10 +7768,10 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C5"/>
+      <selection activeCell="F2" sqref="A1:F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="25.88671875" style="1" bestFit="1" customWidth="1"/>
@@ -7700,7 +7782,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -7720,7 +7802,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>41</v>
       </c>
@@ -7738,7 +7820,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>42</v>
       </c>
@@ -7758,7 +7840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>43</v>
       </c>
@@ -7778,7 +7860,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>44</v>
       </c>
@@ -7813,7 +7895,7 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.21875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31" style="1" customWidth="1"/>
@@ -7824,7 +7906,7 @@
     <col min="7" max="16384" width="8.77734375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -7844,7 +7926,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>46</v>
       </c>
@@ -7864,7 +7946,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>47</v>
       </c>
@@ -7884,7 +7966,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>47</v>
       </c>
@@ -7913,7 +7995,7 @@
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.21875" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="30.109375" style="5" bestFit="1" customWidth="1"/>
@@ -7926,7 +8008,7 @@
     <col min="9" max="16384" width="8.77734375" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>7</v>
       </c>
@@ -7952,7 +8034,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="165.6">
+    <row r="2" spans="1:8" ht="158.4" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>38</v>
       </c>
@@ -7978,7 +8060,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="303.60000000000002">
+    <row r="3" spans="1:8" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
         <v>39</v>
       </c>
@@ -8004,7 +8086,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>40</v>
       </c>
@@ -8026,7 +8108,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
keep add case for sdl-6761
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E6277C-8881-4975-BC40-1F2EA53E83C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D52AC3-47FE-4715-9308-1DFB3ADD2B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-14560" windowWidth="38620" windowHeight="21220" tabRatio="800" firstSheet="6" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -24,10 +24,12 @@
     <sheet name="deleteEntities" sheetId="4" r:id="rId9"/>
     <sheet name="createRelations" sheetId="19" r:id="rId10"/>
     <sheet name="updateRelations" sheetId="20" r:id="rId11"/>
-    <sheet name="listGraphNames" sheetId="24" r:id="rId12"/>
-    <sheet name="getRelationById" sheetId="7" r:id="rId13"/>
-    <sheet name="getRelations" sheetId="6" r:id="rId14"/>
-    <sheet name="deleteRelations" sheetId="16" r:id="rId15"/>
+    <sheet name="getRelationById" sheetId="7" r:id="rId12"/>
+    <sheet name="getRelations" sheetId="6" r:id="rId13"/>
+    <sheet name="deleteRelations" sheetId="16" r:id="rId14"/>
+    <sheet name="listGraphNames" sheetId="24" r:id="rId15"/>
+    <sheet name="createInstanceGraph" sheetId="25" r:id="rId16"/>
+    <sheet name="generateKg" sheetId="26" r:id="rId17"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="403">
   <si>
     <t>testEntity1</t>
   </si>
@@ -3862,11 +3864,60 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>response</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>[ "janusgraph_iot_demo_dev_kg",   "janusgraph_iot_demo_dev_instance_kg"]</t>
+    <t>iot-lpg-create-instance-graph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>create instance graph</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>graphName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>test6761</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>responseData</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>iot-lpg-generate-kg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>generate kg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>entityLabels</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>sdl_b</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>graphql</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>{
+    sdl_b (cond: "", authInfo: "", order: "") {
+        id
+        hobby
+    }
+}</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>janusgraph_iot_demo_dev_kg,test6761,janusgraph_iot_demo_dev_instance_kg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>janusgraph_iot_demo_dev_kg,janusgraph_iot_demo_dev_instance_kg</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -5829,68 +5880,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23BC73A-A0BF-4177-B9E9-728F3C997D3D}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="30.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="34.77734375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
-        <v>388</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>391</v>
-      </c>
-      <c r="D2" s="2">
-        <v>200</v>
-      </c>
-      <c r="E2" s="2">
-        <v>100000</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE8CB3E4-B830-482F-A87D-FE5107D53FAD}">
   <dimension ref="A1:I4"/>
   <sheetViews>
@@ -6023,7 +6012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7825D-C3D3-4455-B765-0D831E376750}">
   <dimension ref="A1:F5"/>
   <sheetViews>
@@ -6147,7 +6136,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C3E9BB9-23BC-452F-AE17-4472AC4F82DB}">
   <dimension ref="A1:I5"/>
   <sheetViews>
@@ -6302,6 +6291,213 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23BC73A-A0BF-4177-B9E9-728F3C997D3D}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24" customWidth="1"/>
+    <col min="3" max="3" width="34.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="26.4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>388</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>402</v>
+      </c>
+      <c r="D2" s="2">
+        <v>200</v>
+      </c>
+      <c r="E2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96E34F12-E0EE-4BEF-A622-8CC26A6B72AF}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="32.44140625" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" customWidth="1"/>
+    <col min="3" max="4" width="19.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="52.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>390</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>401</v>
+      </c>
+      <c r="E2" s="2">
+        <v>200</v>
+      </c>
+      <c r="F2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EC30DF-967B-4F8A-8865-54A6D8527064}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.5546875" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" customWidth="1"/>
+    <col min="3" max="3" width="21.5546875" customWidth="1"/>
+    <col min="4" max="5" width="37" customWidth="1"/>
+    <col min="6" max="6" width="21.21875" customWidth="1"/>
+    <col min="7" max="7" width="18.21875" customWidth="1"/>
+    <col min="8" max="8" width="50.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>398</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>400</v>
+      </c>
+      <c r="F2" s="2">
+        <v>200</v>
+      </c>
+      <c r="G2" s="2">
+        <v>100000</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
add case for sdl-6761
</commit_message>
<xml_diff>
--- a/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
+++ b/src/main/resources/test-data-xls/iot-entity-management-test-data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\auto_worksapce\feature-automation\src\main\resources\test-data-xls\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D52AC3-47FE-4715-9308-1DFB3ADD2B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE33859A-1368-4E6E-B54A-125592061B15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="11" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" tabRatio="800" firstSheet="11" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="publishCheck" sheetId="21" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="772" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="404">
   <si>
     <t>testEntity1</t>
   </si>
@@ -3918,6 +3918,10 @@
   </si>
   <si>
     <t>janusgraph_iot_demo_dev_kg,janusgraph_iot_demo_dev_instance_kg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>instanceNum</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -6300,7 +6304,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B23BC73A-A0BF-4177-B9E9-728F3C997D3D}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
@@ -6427,10 +6431,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EC30DF-967B-4F8A-8865-54A6D8527064}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -6438,13 +6442,13 @@
     <col min="1" max="1" width="28.5546875" customWidth="1"/>
     <col min="2" max="2" width="31.77734375" customWidth="1"/>
     <col min="3" max="3" width="21.5546875" customWidth="1"/>
-    <col min="4" max="5" width="37" customWidth="1"/>
-    <col min="6" max="6" width="21.21875" customWidth="1"/>
-    <col min="7" max="7" width="18.21875" customWidth="1"/>
-    <col min="8" max="8" width="50.44140625" customWidth="1"/>
+    <col min="4" max="6" width="37" customWidth="1"/>
+    <col min="7" max="7" width="21.21875" customWidth="1"/>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="50.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -6461,16 +6465,19 @@
         <v>399</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>403</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="79.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="79.2" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>395</v>
       </c>
@@ -6486,13 +6493,16 @@
       <c r="E2" s="21" t="s">
         <v>400</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="21">
+        <v>2</v>
+      </c>
+      <c r="G2" s="2">
         <v>200</v>
       </c>
-      <c r="G2" s="2">
+      <c r="H2" s="2">
         <v>100000</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>16</v>
       </c>
     </row>

</xml_diff>